<commit_message>
registerverwerking + filterchain opgezet + authenticatie nu met encryptie + authorritiesrepo en -service
</commit_message>
<xml_diff>
--- a/logboek.xlsx
+++ b/logboek.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="42">
   <si>
     <t xml:space="preserve">Naam student 1:</t>
   </si>
@@ -92,6 +92,69 @@
   </si>
   <si>
     <t xml:space="preserve">28/12/2024</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Opzetten van de security</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RestInterface</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Opzetten van de repositories en services</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Databank en services debuggen</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Debuggen van de controllers (afstellen met nieuwe back-end en db)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Project opnieuw beginnen (implementatie werd zeer onoverzichtelijk)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Databank opnieuw ontwerpen</t>
+  </si>
+  <si>
+    <t xml:space="preserve">model opnieuw ontwerpen </t>
+  </si>
+  <si>
+    <t xml:space="preserve">controllers opnieuw ontwerpen</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Services en repositories opnieuw ontwerpen</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HTML pagina’s opnieuw maken</t>
+  </si>
+  <si>
+    <t xml:space="preserve">controllers afwerken</t>
+  </si>
+  <si>
+    <t xml:space="preserve">services afwerken</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HTML verder maken</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">databank aanpassen
+</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">Model aanpassen aan services</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Restinterface</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Security aanpassen</t>
   </si>
 </sst>
 </file>
@@ -104,7 +167,7 @@
     <numFmt numFmtId="166" formatCode="m/d/yyyy"/>
     <numFmt numFmtId="167" formatCode="0.00"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="7">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -133,6 +196,19 @@
       <color theme="3"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val=""/>
+      <family val="1"/>
       <charset val="1"/>
     </font>
   </fonts>
@@ -203,7 +279,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="18">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -242,6 +318,26 @@
     </xf>
     <xf numFmtId="167" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
@@ -506,10 +602,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D57"/>
+  <dimension ref="A1:D63"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A3" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E9" activeCellId="0" sqref="E9"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D40" activeCellId="0" sqref="D40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.55078125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -564,7 +660,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="58.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="57.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="7" t="s">
         <v>8</v>
       </c>
@@ -578,7 +674,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="29.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="7" t="s">
         <v>9</v>
       </c>
@@ -592,7 +688,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="100.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" customFormat="false" ht="99.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="7" t="s">
         <v>10</v>
       </c>
@@ -606,7 +702,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="29.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" customFormat="false" ht="29.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="7" t="s">
         <v>12</v>
       </c>
@@ -620,7 +716,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="29.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" customFormat="false" ht="29.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="7" t="s">
         <v>14</v>
       </c>
@@ -634,7 +730,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="29.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" customFormat="false" ht="29.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="7" t="s">
         <v>16</v>
       </c>
@@ -648,7 +744,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="44" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" customFormat="false" ht="43.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="7" t="s">
         <v>18</v>
       </c>
@@ -662,7 +758,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="58.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="12" customFormat="false" ht="43.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="7" t="s">
         <v>19</v>
       </c>
@@ -676,7 +772,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="58.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="13" customFormat="false" ht="57.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="7" t="s">
         <v>20</v>
       </c>
@@ -690,7 +786,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" customFormat="false" ht="58.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14" customFormat="false" ht="43.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="7" t="s">
         <v>22</v>
       </c>
@@ -710,35 +806,73 @@
       <c r="C15" s="6"/>
       <c r="D15" s="6"/>
     </row>
-    <row r="16" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="7"/>
-      <c r="B16" s="5"/>
-      <c r="C16" s="6"/>
-      <c r="D16" s="6"/>
+    <row r="16" customFormat="false" ht="43.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="B16" s="5" t="n">
+        <v>45689</v>
+      </c>
+      <c r="C16" s="6" t="n">
+        <v>6</v>
+      </c>
+      <c r="D16" s="6" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="17" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="7"/>
-      <c r="B17" s="5"/>
+      <c r="A17" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="B17" s="5" t="n">
+        <v>45689</v>
+      </c>
       <c r="C17" s="6"/>
-      <c r="D17" s="6"/>
+      <c r="D17" s="6" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="18" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="7"/>
-      <c r="B18" s="5"/>
-      <c r="C18" s="6"/>
-      <c r="D18" s="6"/>
-    </row>
-    <row r="19" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="7"/>
-      <c r="B19" s="5"/>
-      <c r="C19" s="6"/>
-      <c r="D19" s="6"/>
-    </row>
-    <row r="20" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="7"/>
-      <c r="B20" s="5"/>
-      <c r="C20" s="6"/>
-      <c r="D20" s="6"/>
+      <c r="A18" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="B18" s="5" t="n">
+        <v>45689</v>
+      </c>
+      <c r="C18" s="6" t="n">
+        <v>3</v>
+      </c>
+      <c r="D18" s="6" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="29.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="B19" s="5" t="n">
+        <v>45689</v>
+      </c>
+      <c r="C19" s="6" t="n">
+        <v>1</v>
+      </c>
+      <c r="D19" s="6" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="29.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="B20" s="5" t="n">
+        <v>45689</v>
+      </c>
+      <c r="C20" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="D20" s="6" t="n">
+        <v>3</v>
+      </c>
     </row>
     <row r="21" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="7"/>
@@ -746,23 +880,47 @@
       <c r="C21" s="6"/>
       <c r="D21" s="6"/>
     </row>
-    <row r="22" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="7"/>
-      <c r="B22" s="5"/>
-      <c r="C22" s="6"/>
-      <c r="D22" s="6"/>
-    </row>
-    <row r="23" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="7"/>
-      <c r="B23" s="5"/>
-      <c r="C23" s="6"/>
-      <c r="D23" s="6"/>
+    <row r="22" customFormat="false" ht="43.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="B22" s="5" t="n">
+        <v>45717</v>
+      </c>
+      <c r="C22" s="6" t="n">
+        <v>6</v>
+      </c>
+      <c r="D22" s="6" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="29.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="B23" s="5" t="n">
+        <v>45717</v>
+      </c>
+      <c r="C23" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="D23" s="6" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="24" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="7"/>
-      <c r="B24" s="5"/>
-      <c r="C24" s="6"/>
-      <c r="D24" s="6"/>
+      <c r="A24" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="B24" s="5" t="n">
+        <v>45717</v>
+      </c>
+      <c r="C24" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="D24" s="6" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="25" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="7"/>
@@ -770,186 +928,326 @@
       <c r="C25" s="6"/>
       <c r="D25" s="6"/>
     </row>
-    <row r="26" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="7"/>
-      <c r="B26" s="5"/>
-      <c r="C26" s="6"/>
-      <c r="D26" s="6"/>
+    <row r="26" customFormat="false" ht="43.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="B26" s="5" t="n">
+        <v>45717</v>
+      </c>
+      <c r="C26" s="6" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="D26" s="6" t="n">
+        <v>0.5</v>
+      </c>
     </row>
     <row r="27" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="7"/>
-      <c r="B27" s="5"/>
-      <c r="C27" s="6"/>
-      <c r="D27" s="6"/>
+      <c r="A27" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="B27" s="5" t="n">
+        <v>45717</v>
+      </c>
+      <c r="C27" s="6" t="n">
+        <v>1</v>
+      </c>
+      <c r="D27" s="6" t="n">
+        <v>3</v>
+      </c>
     </row>
     <row r="28" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="7"/>
-      <c r="B28" s="5"/>
-      <c r="C28" s="6"/>
-      <c r="D28" s="6"/>
+      <c r="A28" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="B28" s="5" t="n">
+        <v>45717</v>
+      </c>
+      <c r="C28" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="D28" s="6" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="29" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="7"/>
-      <c r="B29" s="5"/>
-      <c r="C29" s="6"/>
-      <c r="D29" s="6"/>
-    </row>
-    <row r="30" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="7"/>
-      <c r="B30" s="5"/>
-      <c r="C30" s="6"/>
-      <c r="D30" s="6"/>
+      <c r="A29" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="B29" s="5" t="n">
+        <v>45717</v>
+      </c>
+      <c r="C29" s="6" t="n">
+        <v>5</v>
+      </c>
+      <c r="D29" s="6" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="29.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="B30" s="5" t="n">
+        <v>45717</v>
+      </c>
+      <c r="C30" s="6" t="n">
+        <v>1</v>
+      </c>
+      <c r="D30" s="6" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="31" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="7"/>
-      <c r="B31" s="5"/>
-      <c r="C31" s="6"/>
-      <c r="D31" s="6"/>
+      <c r="A31" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="B31" s="5" t="n">
+        <v>45717</v>
+      </c>
+      <c r="C31" s="6" t="n">
+        <v>1</v>
+      </c>
+      <c r="D31" s="6" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="32" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="7"/>
-      <c r="B32" s="5"/>
+      <c r="A32" s="0"/>
+      <c r="B32" s="12"/>
       <c r="C32" s="6"/>
       <c r="D32" s="6"/>
     </row>
     <row r="33" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="7"/>
-      <c r="B33" s="5"/>
-      <c r="C33" s="6"/>
-      <c r="D33" s="6"/>
+      <c r="A33" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="B33" s="12" t="n">
+        <v>45748</v>
+      </c>
+      <c r="C33" s="6" t="n">
+        <v>7</v>
+      </c>
+      <c r="D33" s="6" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="34" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="10"/>
-      <c r="B34" s="11"/>
-      <c r="C34" s="12" t="n">
-        <f aca="false">SUM(C4:C33)</f>
-        <v>13.5</v>
-      </c>
-      <c r="D34" s="12" t="n">
-        <f aca="false">SUM(D4:D33)</f>
-        <v>12</v>
+      <c r="A34" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="B34" s="12" t="n">
+        <v>45748</v>
+      </c>
+      <c r="C34" s="6" t="n">
+        <v>2</v>
+      </c>
+      <c r="D34" s="6" t="n">
+        <v>3</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="10"/>
-      <c r="B35" s="11"/>
-      <c r="C35" s="12"/>
-      <c r="D35" s="12"/>
-    </row>
-    <row r="36" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="10"/>
-      <c r="B36" s="11"/>
-      <c r="C36" s="12"/>
-      <c r="D36" s="12"/>
+      <c r="A35" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="B35" s="12" t="n">
+        <v>45748</v>
+      </c>
+      <c r="C35" s="6" t="n">
+        <v>1</v>
+      </c>
+      <c r="D35" s="6" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" customFormat="false" ht="43.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A36" s="13" t="s">
+        <v>38</v>
+      </c>
+      <c r="B36" s="12" t="n">
+        <v>45748</v>
+      </c>
+      <c r="C36" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="D36" s="6" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="37" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="10"/>
-      <c r="B37" s="11"/>
-      <c r="C37" s="12"/>
-      <c r="D37" s="12"/>
+      <c r="A37" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="B37" s="12" t="n">
+        <v>45748</v>
+      </c>
+      <c r="C37" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="D37" s="6" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="38" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A38" s="10"/>
-      <c r="B38" s="11"/>
-      <c r="C38" s="12"/>
-      <c r="D38" s="12"/>
+      <c r="A38" s="14" t="s">
+        <v>40</v>
+      </c>
+      <c r="B38" s="12" t="n">
+        <v>45748</v>
+      </c>
+      <c r="C38" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="D38" s="6" t="n">
+        <v>3</v>
+      </c>
     </row>
     <row r="39" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A39" s="10"/>
-      <c r="B39" s="11"/>
-      <c r="C39" s="12"/>
-      <c r="D39" s="12"/>
+      <c r="A39" s="14" t="s">
+        <v>41</v>
+      </c>
+      <c r="B39" s="12" t="n">
+        <v>45748</v>
+      </c>
+      <c r="C39" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="D39" s="6" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="40" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A40" s="10"/>
-      <c r="B40" s="11"/>
-      <c r="C40" s="12"/>
-      <c r="D40" s="12"/>
+      <c r="A40" s="15"/>
+      <c r="B40" s="16"/>
+      <c r="C40" s="17" t="n">
+        <f aca="false">SUM(C4:C39)</f>
+        <v>48</v>
+      </c>
+      <c r="D40" s="17" t="n">
+        <f aca="false">SUM(D4:D39)</f>
+        <v>48.5</v>
+      </c>
     </row>
     <row r="41" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A41" s="10"/>
-      <c r="B41" s="11"/>
-      <c r="C41" s="12"/>
-      <c r="D41" s="12"/>
+      <c r="A41" s="15"/>
+      <c r="B41" s="16"/>
+      <c r="C41" s="17"/>
+      <c r="D41" s="17"/>
     </row>
     <row r="42" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A42" s="10"/>
-      <c r="B42" s="11"/>
-      <c r="C42" s="12"/>
-      <c r="D42" s="12"/>
+      <c r="A42" s="15"/>
+      <c r="B42" s="16"/>
+      <c r="C42" s="17"/>
+      <c r="D42" s="17"/>
     </row>
     <row r="43" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A43" s="10"/>
-      <c r="B43" s="11"/>
-      <c r="C43" s="12"/>
-      <c r="D43" s="12"/>
+      <c r="A43" s="15"/>
+      <c r="B43" s="16"/>
+      <c r="C43" s="17"/>
+      <c r="D43" s="17"/>
     </row>
     <row r="44" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A44" s="10"/>
-      <c r="B44" s="11"/>
-      <c r="C44" s="12"/>
-      <c r="D44" s="12"/>
+      <c r="A44" s="15"/>
+      <c r="B44" s="16"/>
+      <c r="C44" s="17"/>
+      <c r="D44" s="17"/>
     </row>
     <row r="45" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A45" s="10"/>
-      <c r="B45" s="11"/>
-      <c r="C45" s="12"/>
-      <c r="D45" s="12"/>
+      <c r="A45" s="15"/>
+      <c r="B45" s="16"/>
+      <c r="C45" s="17"/>
+      <c r="D45" s="17"/>
     </row>
     <row r="46" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A46" s="10"/>
-      <c r="B46" s="11"/>
-      <c r="C46" s="12"/>
-      <c r="D46" s="12"/>
+      <c r="A46" s="15"/>
+      <c r="B46" s="16"/>
+      <c r="C46" s="17"/>
+      <c r="D46" s="17"/>
     </row>
     <row r="47" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B47" s="11"/>
-      <c r="C47" s="12"/>
-      <c r="D47" s="12"/>
+      <c r="A47" s="15"/>
+      <c r="B47" s="16"/>
+      <c r="C47" s="17"/>
+      <c r="D47" s="17"/>
     </row>
     <row r="48" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B48" s="11"/>
-      <c r="C48" s="12"/>
-      <c r="D48" s="12"/>
+      <c r="A48" s="15"/>
+      <c r="B48" s="16"/>
+      <c r="C48" s="17"/>
+      <c r="D48" s="17"/>
     </row>
     <row r="49" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B49" s="11"/>
-      <c r="C49" s="12"/>
-      <c r="D49" s="12"/>
+      <c r="A49" s="15"/>
+      <c r="B49" s="16"/>
+      <c r="C49" s="17"/>
+      <c r="D49" s="17"/>
     </row>
     <row r="50" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B50" s="11"/>
-      <c r="C50" s="12"/>
-      <c r="D50" s="12"/>
+      <c r="A50" s="15"/>
+      <c r="B50" s="16"/>
+      <c r="C50" s="17"/>
+      <c r="D50" s="17"/>
     </row>
     <row r="51" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B51" s="11"/>
-      <c r="C51" s="12"/>
-      <c r="D51" s="12"/>
+      <c r="A51" s="15"/>
+      <c r="B51" s="16"/>
+      <c r="C51" s="17"/>
+      <c r="D51" s="17"/>
     </row>
     <row r="52" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B52" s="11"/>
-      <c r="C52" s="12"/>
-      <c r="D52" s="12"/>
+      <c r="A52" s="15"/>
+      <c r="B52" s="16"/>
+      <c r="C52" s="17"/>
+      <c r="D52" s="17"/>
     </row>
     <row r="53" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B53" s="11"/>
-      <c r="C53" s="12"/>
-      <c r="D53" s="12"/>
+      <c r="B53" s="16"/>
+      <c r="C53" s="17"/>
+      <c r="D53" s="17"/>
     </row>
     <row r="54" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B54" s="11"/>
-      <c r="C54" s="12"/>
-      <c r="D54" s="12"/>
+      <c r="B54" s="16"/>
+      <c r="C54" s="17"/>
+      <c r="D54" s="17"/>
     </row>
     <row r="55" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D55" s="12"/>
+      <c r="B55" s="16"/>
+      <c r="C55" s="17"/>
+      <c r="D55" s="17"/>
     </row>
     <row r="56" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D56" s="12"/>
+      <c r="B56" s="16"/>
+      <c r="C56" s="17"/>
+      <c r="D56" s="17"/>
     </row>
     <row r="57" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D57" s="12"/>
+      <c r="B57" s="16"/>
+      <c r="C57" s="17"/>
+      <c r="D57" s="17"/>
+    </row>
+    <row r="58" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B58" s="16"/>
+      <c r="C58" s="17"/>
+      <c r="D58" s="17"/>
+    </row>
+    <row r="59" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B59" s="16"/>
+      <c r="C59" s="17"/>
+      <c r="D59" s="17"/>
+    </row>
+    <row r="60" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B60" s="16"/>
+      <c r="C60" s="17"/>
+      <c r="D60" s="17"/>
+    </row>
+    <row r="61" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D61" s="17"/>
+    </row>
+    <row r="62" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D62" s="17"/>
+    </row>
+    <row r="63" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D63" s="17"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>